<commit_message>
First commit after reinit
</commit_message>
<xml_diff>
--- a/docs/Extensions.xlsx
+++ b/docs/Extensions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dane\VS\Projects\MyLib\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6816DB56-F427-426C-B7F6-916F9EB3830C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED31548-70C1-421E-9607-50BED15C2A4F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9660" activeTab="2" xr2:uid="{EE045EA3-223E-4C82-A696-7376FC666CEC}"/>
   </bookViews>
@@ -21497,7 +21497,7 @@
   <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:XFD46"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>